<commit_message>
add correction of midterm fall 2016
</commit_message>
<xml_diff>
--- a/files/QT/midterm_oct2016_CORRECT.xlsx
+++ b/files/QT/midterm_oct2016_CORRECT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Section 1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>Alice</t>
   </si>
@@ -191,12 +191,6 @@
     <t>4. Compute the Laspeyres index in 2015 using 2012 as a baseline year</t>
   </si>
   <si>
-    <t>PRICES</t>
-  </si>
-  <si>
-    <t>QUANTITIES</t>
-  </si>
-  <si>
     <t>5. Compute the Paasche index in 2015 using 2012 as a baseline year</t>
   </si>
   <si>
@@ -222,17 +216,22 @@
   </si>
   <si>
     <t>6. What should be the flat tax-rate so that Alice the same amount of taxes ?</t>
+  </si>
+  <si>
+    <t>Quantities</t>
+  </si>
+  <si>
+    <t>Prices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,8 +263,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,8 +285,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -287,8 +312,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -324,18 +358,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -343,9 +399,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -363,6 +450,19 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -380,6 +480,19 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,17 +828,17 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -735,40 +848,40 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="17">
         <f>2*1.2</f>
         <v>2.4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="19">
         <f>4/(1.2)</f>
         <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="18">
         <f>(1.15-1.2)/1.2</f>
         <v>-4.1666666666666706E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -776,27 +889,28 @@
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="18">
         <f>(1.05*1.1*1.02)^(1/3)-1</f>
         <v>5.6154333503796838E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="7">
+      <c r="B10" s="21">
         <f>LN(5)/LN(1.05)</f>
         <v>32.986933736173881</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="20" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -810,10 +924,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -827,41 +941,41 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="B2" s="3">
+      <c r="B2" s="16">
         <v>1200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" s="8" customFormat="1">
-      <c r="A4" s="8" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" s="4" customFormat="1">
+      <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="17">
         <f>B2*1.2</f>
         <v>1440</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="A6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="17">
         <f>B2*1.3</f>
         <v>1560</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="A7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="18">
         <f>(B5-B6)/B6</f>
         <v>-7.6923076923076927E-2</v>
       </c>
@@ -870,58 +984,59 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" s="8" customFormat="1">
-      <c r="A9" s="8" t="s">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" s="4" customFormat="1">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="A10" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2">
+      <c r="B10" s="22"/>
+      <c r="C10" s="18">
         <f>(B6-B5)/B5</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="22" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" s="8" customFormat="1">
-      <c r="A12" s="8" t="s">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" s="4" customFormat="1">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="18">
         <f>1.02^3-1</f>
         <v>6.1207999999999929E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" s="10" customFormat="1">
-      <c r="A15" s="10" t="s">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" s="6" customFormat="1">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="18">
         <f>1.2/(1.02^3)-1</f>
         <v>0.13078680145645349</v>
       </c>
@@ -930,25 +1045,25 @@
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="18">
         <f>1.3/(1.02^3)-1</f>
         <v>0.22501903491115804</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" s="8" customFormat="1">
-      <c r="A19" s="8" t="s">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" s="4" customFormat="1">
+      <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="17">
         <f>0.05*500+0.15*500+0.2*60</f>
         <v>112</v>
       </c>
@@ -957,27 +1072,27 @@
       <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="23">
         <f>0.05*500+0.15*440</f>
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="8" customFormat="1">
-      <c r="A23" s="8" t="s">
-        <v>66</v>
+    <row r="23" spans="1:3" s="4" customFormat="1">
+      <c r="A23" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="18">
         <f>C21/B5</f>
         <v>6.3194444444444442E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="8" customFormat="1">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:3" s="4" customFormat="1">
+      <c r="A26" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -990,13 +1105,13 @@
       <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="24">
         <f>1400+(9-5)/(9-5+9-4)*200</f>
         <v>1488.8888888888889</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="8" customFormat="1">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:3" s="4" customFormat="1">
+      <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1020,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1032,7 +1147,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1044,7 +1159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1056,24 +1171,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C37">
-        <f>1400+200*(11-5)/14</f>
-        <v>1485.7142857142858</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="24">
+        <f>1400+200*(11-C32)/B33</f>
+        <v>1533.3333333333333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="D39" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1090,114 +1209,119 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF0000FF"/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="6.83203125" customWidth="1"/>
+    <col min="5" max="5" width="2.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="A3" s="13">
         <v>0.6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" s="13">
         <v>0.35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="A5" s="13">
         <v>0.05</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="8" customFormat="1">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:4" s="4" customFormat="1">
+      <c r="A7" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="A9" s="13">
         <v>2013</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="13">
         <v>5</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="13">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="13">
         <v>-3</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="A10" s="13">
         <v>2014</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="13">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="13">
         <v>4</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
+      <c r="A11" s="13">
         <v>2015</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="13">
         <v>3</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="13">
         <v>2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="8" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1205,13 +1329,13 @@
       <c r="A14">
         <v>2012</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="8">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="8">
         <v>1</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1219,15 +1343,15 @@
       <c r="A15">
         <v>2013</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="24">
         <f t="shared" ref="B15:D17" si="0">B14*(1+B9/100)</f>
         <v>1.05</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="24">
         <f t="shared" si="0"/>
         <v>1.02</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="24">
         <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
@@ -1236,42 +1360,42 @@
       <c r="A16">
         <v>2014</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="24">
         <f t="shared" si="0"/>
         <v>1.0605</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="24">
         <f t="shared" si="0"/>
         <v>1.0608</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="24">
         <f t="shared" si="0"/>
         <v>0.98939999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>2015</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="24">
         <f t="shared" si="0"/>
         <v>1.0923149999999999</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="24">
         <f t="shared" si="0"/>
         <v>1.0820160000000001</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="24">
         <f t="shared" si="0"/>
         <v>1.0289759999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="8" customFormat="1">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:9" s="4" customFormat="1">
+      <c r="A19" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:9">
       <c r="B20" t="s">
         <v>52</v>
       </c>
@@ -1279,7 +1403,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>2012</v>
       </c>
@@ -1288,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>2013</v>
       </c>
@@ -1296,12 +1420,12 @@
         <f>B15*$A$3+C15*$A$4+D15*$A$5</f>
         <v>1.0355000000000001</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="18">
         <f>(B22-B21)/B21</f>
         <v>3.5500000000000087E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>2014</v>
       </c>
@@ -1309,12 +1433,12 @@
         <f t="shared" ref="B23:B24" si="1">B16*$A$3+C16*$A$4+D16*$A$5</f>
         <v>1.0570499999999998</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="18">
         <f t="shared" ref="C23:C24" si="2">(B23-B22)/B22</f>
         <v>2.0811202317720653E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>2015</v>
       </c>
@@ -1322,233 +1446,258 @@
         <f t="shared" si="1"/>
         <v>1.0855433999999999</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="18">
         <f t="shared" si="2"/>
         <v>2.6955583936426959E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="8" customFormat="1">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:9" s="4" customFormat="1">
+      <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2">
+    <row r="27" spans="1:9">
+      <c r="A27" s="1">
         <f>((1+C22)*(1+C23)*(1+C24))^(1/3)-1</f>
         <v>2.7737958514654215E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="B28" s="12" t="s">
+    <row r="28" spans="1:9">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" s="10" customFormat="1">
+      <c r="A29" s="9"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D31" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="B29" s="12" t="s">
+      <c r="E31" s="13"/>
+      <c r="F31" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="13">
+        <v>2012</v>
+      </c>
+      <c r="B32" s="15">
+        <v>100</v>
+      </c>
+      <c r="C32" s="15">
+        <v>40</v>
+      </c>
+      <c r="D32" s="15">
+        <v>6</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13">
+        <v>2012</v>
+      </c>
+      <c r="G32" s="13">
+        <v>2.9</v>
+      </c>
+      <c r="H32" s="13">
+        <v>10.3</v>
+      </c>
+      <c r="I32" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="13">
+        <v>2015</v>
+      </c>
+      <c r="B33" s="15">
+        <f>B32*1.15</f>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="C33" s="15">
+        <f>C32*0.9</f>
+        <v>36</v>
+      </c>
+      <c r="D33" s="15">
+        <f>D32</f>
+        <v>6</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13">
+        <v>2013</v>
+      </c>
+      <c r="G33" s="13">
+        <v>3</v>
+      </c>
+      <c r="H33" s="13">
+        <v>10</v>
+      </c>
+      <c r="I33" s="13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13">
+        <v>2014</v>
+      </c>
+      <c r="G34" s="13">
+        <v>3.2</v>
+      </c>
+      <c r="H34" s="13">
+        <v>10.5</v>
+      </c>
+      <c r="I34" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13">
+        <v>2015</v>
+      </c>
+      <c r="G35" s="13">
+        <v>3.3</v>
+      </c>
+      <c r="H35" s="13">
+        <v>10.8</v>
+      </c>
+      <c r="I35" s="13">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="4" customFormat="1">
+      <c r="A38" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="25">
+        <f>(G35*B32+H35*C32+I35*D32)/(B32*G32+C32*H32+D32*I32)*100</f>
+        <v>108.55207451312448</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="4" customFormat="1">
+      <c r="A41" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="25">
+        <f>SUMPRODUCT(B33:D33,G35:I35)/SUMPRODUCT(B33:D33,G32:I32)*100</f>
+        <v>109.08707272471516</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
-        <v>2012</v>
-      </c>
-      <c r="B30" s="12">
-        <v>100</v>
-      </c>
-      <c r="C30" s="12">
-        <v>40</v>
-      </c>
-      <c r="D30" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
+      <c r="C44" s="13"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="13">
+        <v>2013</v>
+      </c>
+      <c r="B45" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="C45" s="13"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="13">
+        <v>2014</v>
+      </c>
+      <c r="B46" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="13">
         <v>2015</v>
       </c>
-      <c r="B31" s="12">
-        <f>B30*1.15</f>
-        <v>114.99999999999999</v>
-      </c>
-      <c r="C31" s="12">
-        <f>C30*0.9</f>
-        <v>36</v>
-      </c>
-      <c r="D31" s="12">
-        <f>D30</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="B32" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33">
-        <v>2012</v>
-      </c>
-      <c r="B33">
-        <v>2.9</v>
-      </c>
-      <c r="C33">
-        <v>10.3</v>
-      </c>
-      <c r="D33">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34">
-        <v>2013</v>
-      </c>
-      <c r="B34">
-        <v>3</v>
-      </c>
-      <c r="C34">
-        <v>10</v>
-      </c>
-      <c r="D34">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35">
-        <v>2014</v>
-      </c>
-      <c r="B35">
-        <v>3.2</v>
-      </c>
-      <c r="C35">
-        <v>10.5</v>
-      </c>
-      <c r="D35">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36">
-        <v>2015</v>
-      </c>
-      <c r="B36">
-        <v>3.3</v>
-      </c>
-      <c r="C36">
-        <v>10.8</v>
-      </c>
-      <c r="D36">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="8" customFormat="1">
-      <c r="A39" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="5">
-        <f>(B36*B30+C36*C30+D36*D30)/(B30*B33+C30*C33+D30*D33)</f>
-        <v>1.0855207451312447</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="8" customFormat="1">
-      <c r="A42" s="8" t="s">
+      <c r="B47" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="C47" s="13"/>
+    </row>
+    <row r="49" spans="1:6" s="4" customFormat="1">
+      <c r="A49" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="5">
-        <f>SUMPRODUCT(B31:D31,B36:D36)/SUMPRODUCT(B31:D31,B33:D33)</f>
-        <v>1.0908707272471516</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="B45" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46">
-        <v>2013</v>
-      </c>
-      <c r="B46">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47">
-        <v>2014</v>
-      </c>
-      <c r="B47">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48">
-        <v>2015</v>
-      </c>
-      <c r="B48">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="8" customFormat="1">
-      <c r="A50" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="1">
+    <row r="50" spans="1:6">
+      <c r="A50" s="18">
         <f xml:space="preserve"> (1.015*1.008*1.007)^(1/3)-1</f>
         <v>9.993739137087454E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="8" customFormat="1">
-      <c r="A53" s="8" t="s">
+    <row r="52" spans="1:6" s="4" customFormat="1">
+      <c r="A52" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="B53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="B54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="B55">
-        <f>(1+A51)^3</f>
+    <row r="54" spans="1:6">
+      <c r="B54">
+        <f>(1+A50)^3</f>
         <v>1.0302818399999996</v>
       </c>
-      <c r="C55">
+      <c r="C54">
         <f>B24*650</f>
         <v>705.60320999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>64</v>
-      </c>
-      <c r="D57" s="6">
-        <f>C55/B55</f>
+    <row r="55" spans="1:6" s="2" customFormat="1">
+      <c r="A55" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="26">
+        <f>C54/B54</f>
         <v>684.86426005528767</v>
       </c>
-      <c r="E57" t="s">
-        <v>65</v>
-      </c>
+      <c r="E55" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F55" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>